<commit_message>
Rounding out excel models and adding readme links
</commit_message>
<xml_diff>
--- a/03. Advanced Lookups.xlsx
+++ b/03. Advanced Lookups.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="62">
   <si>
     <t>Gross Sales</t>
   </si>
@@ -212,6 +212,12 @@
   <si>
     <t>CoGS as % of Sales</t>
   </si>
+  <si>
+    <t>This file demonstrates using the INDRECT() function in conjunction with the OFFSET() and MATCH() functions to summarize fictional financial data stored across multiple tabs.</t>
+  </si>
+  <si>
+    <t>This allows for simplified analysis of data which can otherwise be problematic to gather and summarize.</t>
+  </si>
 </sst>
 </file>
 
@@ -220,9 +226,9 @@
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -366,27 +372,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -399,7 +405,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -684,11 +690,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -821,6 +825,16 @@
       <c r="H4" s="26">
         <f t="shared" ca="1" si="0"/>
         <v>0.18856726172792829</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1139,15 +1153,15 @@
       </c>
       <c r="C11" s="7">
         <f t="shared" ref="C11:N11" ca="1" si="1">RANDBETWEEN(18,23)/100*C5</f>
-        <v>251.46</v>
+        <v>228.60000000000002</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>257.37</v>
+        <v>223.8</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>263.40000000000003</v>
+        <v>289.74</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" ca="1" si="1"/>
@@ -1155,11 +1169,11 @@
       </c>
       <c r="G11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>322.56</v>
+        <v>291.84000000000003</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>286.92</v>
+        <v>350.68</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" ca="1" si="1"/>
@@ -1167,11 +1181,11 @@
       </c>
       <c r="J11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>216.72</v>
+        <v>276.92</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>197.03</v>
+        <v>228.14000000000001</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" ca="1" si="1"/>
@@ -1179,11 +1193,11 @@
       </c>
       <c r="M11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>217.44</v>
+        <v>253.67999999999998</v>
       </c>
       <c r="N11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>287.2</v>
+        <v>301.56</v>
       </c>
       <c r="O11" s="15">
         <v>3175</v>
@@ -3410,7 +3424,7 @@
         <v>41640</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:N4" si="0">EOMONTH(C3,0)+1</f>
+        <f t="shared" ref="D3:N3" si="0">EOMONTH(C3,0)+1</f>
         <v>41671</v>
       </c>
       <c r="E3" s="3">
@@ -3656,51 +3670,51 @@
       </c>
       <c r="C11" s="7">
         <f t="shared" ref="C11:N11" ca="1" si="1">RANDBETWEEN(18,23)/100*C5</f>
-        <v>256.68</v>
+        <v>327.98</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>286.02</v>
+        <v>272.40000000000003</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>308.2</v>
+        <v>281.39999999999998</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>225.72</v>
+        <v>184.68</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>199.88</v>
+        <v>189.35999999999999</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>248.22</v>
+        <v>271.86</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>251.24</v>
+        <v>228.4</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>218.4</v>
+        <v>229.32</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>295.8</v>
+        <v>340.17</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>233.64</v>
+        <v>259.60000000000002</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>278.03999999999996</v>
+        <v>304.52000000000004</v>
       </c>
       <c r="N11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>283.14</v>
+        <v>330.33</v>
       </c>
       <c r="O11" s="15">
         <v>3059.2000000000003</v>
@@ -5924,7 +5938,7 @@
         <v>42005</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:N4" si="0">EOMONTH(C3,0)+1</f>
+        <f t="shared" ref="D3:N3" si="0">EOMONTH(C3,0)+1</f>
         <v>42036</v>
       </c>
       <c r="E3" s="3">
@@ -6170,7 +6184,7 @@
       </c>
       <c r="C11" s="7">
         <f t="shared" ref="C11:N11" ca="1" si="1">RANDBETWEEN(18,23)/100*C5</f>
-        <v>303.60000000000002</v>
+        <v>333.96</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" ca="1" si="1"/>
@@ -6178,15 +6192,15 @@
       </c>
       <c r="E11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>219.45</v>
+        <v>207.9</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>333.27</v>
+        <v>349.14</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>355.12</v>
+        <v>293.36</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" ca="1" si="1"/>
@@ -6194,27 +6208,27 @@
       </c>
       <c r="I11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>219.03</v>
+        <v>229.46</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>270</v>
+        <v>283.5</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>333.27000000000004</v>
+        <v>275.31</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>198.55</v>
+        <v>240.35000000000002</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>234.60000000000002</v>
+        <v>224.4</v>
       </c>
       <c r="N11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>328.02</v>
+        <v>342.93</v>
       </c>
       <c r="O11" s="15">
         <v>3166.4</v>
@@ -8438,7 +8452,7 @@
         <v>42370</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:N4" si="0">EOMONTH(C3,0)+1</f>
+        <f t="shared" ref="D3:N3" si="0">EOMONTH(C3,0)+1</f>
         <v>42401</v>
       </c>
       <c r="E3" s="3">
@@ -8684,15 +8698,15 @@
       </c>
       <c r="C11" s="7">
         <f t="shared" ref="C11:N11" ca="1" si="1">RANDBETWEEN(18,23)/100*C5</f>
-        <v>267.95</v>
+        <v>209.7</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>302.82</v>
+        <v>259.56</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>248.01</v>
+        <v>259.82</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" ca="1" si="1"/>
@@ -8700,15 +8714,15 @@
       </c>
       <c r="G11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>224.48999999999998</v>
+        <v>245.87</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>246.06</v>
+        <v>259.73</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>312.8</v>
+        <v>299.2</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" ca="1" si="1"/>
@@ -8716,7 +8730,7 @@
       </c>
       <c r="K11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>233.20000000000002</v>
+        <v>221.54</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" ca="1" si="1"/>
@@ -8724,11 +8738,11 @@
       </c>
       <c r="M11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>243.6</v>
+        <v>220.4</v>
       </c>
       <c r="N11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>188.28</v>
+        <v>240.58</v>
       </c>
       <c r="O11" s="15">
         <v>2878.2</v>
@@ -10952,7 +10966,7 @@
         <v>42736</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:N4" si="0">EOMONTH(C3,0)+1</f>
+        <f t="shared" ref="D3:N3" si="0">EOMONTH(C3,0)+1</f>
         <v>42767</v>
       </c>
       <c r="E3" s="3">
@@ -11198,7 +11212,7 @@
       </c>
       <c r="C11" s="7">
         <f t="shared" ref="C11:N11" ca="1" si="1">RANDBETWEEN(18,23)/100*C5</f>
-        <v>323.39999999999998</v>
+        <v>308.7</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" ca="1" si="1"/>
@@ -11206,43 +11220,43 @@
       </c>
       <c r="E11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>222.42</v>
+        <v>232.53</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>190.79999999999998</v>
+        <v>233.2</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>199.44</v>
+        <v>210.52</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>201.60000000000002</v>
+        <v>231.84</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>338.36</v>
+        <v>353.74</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>295.68</v>
+        <v>267.52</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>282.24</v>
+        <v>255.36</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>237.59</v>
+        <v>196.27</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>219.26</v>
+        <v>207.72</v>
       </c>
       <c r="N11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>264.29000000000002</v>
+        <v>278.2</v>
       </c>
       <c r="O11" s="15">
         <v>2946.2</v>
@@ -13466,7 +13480,7 @@
         <v>43101</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:N4" si="0">EOMONTH(C3,0)+1</f>
+        <f t="shared" ref="D3:N3" si="0">EOMONTH(C3,0)+1</f>
         <v>43132</v>
       </c>
       <c r="E3" s="3">
@@ -13712,11 +13726,11 @@
       </c>
       <c r="C11" s="7">
         <f t="shared" ref="C11:N11" ca="1" si="1">RANDBETWEEN(18,23)/100*C5</f>
-        <v>334.65000000000003</v>
+        <v>291</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>236.34</v>
+        <v>275.73</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" ca="1" si="1"/>
@@ -13724,39 +13738,39 @@
       </c>
       <c r="F11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>249.09</v>
+        <v>288.42</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>292.60000000000002</v>
+        <v>263.33999999999997</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>303.38</v>
+        <v>289.58999999999997</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>325.45</v>
+        <v>311.3</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>295.64</v>
+        <v>342.32</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>271.51</v>
+        <v>257.21999999999997</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>309.98</v>
+        <v>324.07</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>355.58000000000004</v>
+        <v>309.20000000000005</v>
       </c>
       <c r="N11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>229.53</v>
+        <v>218.60000000000002</v>
       </c>
       <c r="O11" s="15">
         <v>3374.4</v>
@@ -16226,43 +16240,43 @@
       </c>
       <c r="C11" s="7">
         <f t="shared" ref="C11:N11" ca="1" si="1">RANDBETWEEN(18,23)/100*C5</f>
-        <v>197.41</v>
+        <v>207.8</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>317.8</v>
+        <v>333.69</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>236.88</v>
+        <v>225.60000000000002</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>271.08</v>
+        <v>301.2</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>201</v>
+        <v>211.04999999999998</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>202.60000000000002</v>
+        <v>222.86</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>268.87</v>
+        <v>233.8</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>258.71999999999997</v>
+        <v>283.36</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>272.33999999999997</v>
+        <v>287.47000000000003</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" ca="1" si="1"/>
@@ -16270,7 +16284,7 @@
       </c>
       <c r="N11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>216.79</v>
+        <v>251.02</v>
       </c>
       <c r="O11" s="15">
         <v>3034.9999999999995</v>

</xml_diff>